<commit_message>
conceptual lca model without mirrored flows sets: done
</commit_message>
<xml_diff>
--- a/default/3 - lca/model/sets.xlsx
+++ b/default/3 - lca/model/sets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\loren\Documents\GitHub\pyesm\default\3 - lca\model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F515C5C-DD57-42B3-9C51-F4248A3AF03B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A7F166-EE73-455C-BAC4-08CC8206822D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="_set_SCENARIOS" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>scen_Names</t>
   </si>
@@ -81,9 +81,6 @@
   </si>
   <si>
     <t>fossil fuels</t>
-  </si>
-  <si>
-    <t>flows_to</t>
   </si>
 </sst>
 </file>
@@ -453,8 +450,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,51 +561,36 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>17</v>
       </c>
-      <c r="B4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>